<commit_message>
Support for U/S32 data in CAN and in USART. User button activates CAN speed check sequence to detect correct CAN speed.
</commit_message>
<xml_diff>
--- a/Software/LowLevel/Documents/bit time.xlsx
+++ b/Software/LowLevel/Documents/bit time.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="24">
   <si>
     <t>CAN bit timing on STM32 F4 Discovery kit</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>APB2 clokc is system clock / prescale -&gt; 48 Mhz / 2 -&gt; 24 Mhz</t>
+  </si>
+  <si>
+    <t>sample point %</t>
   </si>
 </sst>
 </file>
@@ -461,7 +464,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +500,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="K6" t="s">
         <v>14</v>
@@ -515,8 +518,8 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <f>(B6+1)*1/42</f>
-        <v>1</v>
+        <f>(B6+1)*1/84</f>
+        <v>0.69047619047619047</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -557,7 +560,7 @@
       </c>
       <c r="F9" s="4">
         <f>B7+B11+B15</f>
-        <v>8</v>
+        <v>8.2857142857142847</v>
       </c>
       <c r="G9" t="s">
         <v>3</v>
@@ -577,7 +580,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -586,7 +589,7 @@
       </c>
       <c r="B11">
         <f>B10*B7</f>
-        <v>5</v>
+        <v>4.833333333333333</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -600,7 +603,10 @@
         <v>9</v>
       </c>
       <c r="B14" s="1">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -609,7 +615,11 @@
       </c>
       <c r="B15">
         <f>B14*B7</f>
-        <v>2</v>
+        <v>2.7619047619047619</v>
+      </c>
+      <c r="D15">
+        <f>(B11+B7)/(B7+B11+B15)</f>
+        <v>0.66666666666666674</v>
       </c>
     </row>
   </sheetData>
@@ -623,7 +633,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,6 +774,9 @@
       <c r="B14" s="1">
         <v>2</v>
       </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -772,6 +785,10 @@
       <c r="B15">
         <f>B14*B7</f>
         <v>2.75</v>
+      </c>
+      <c r="D15">
+        <f>(B11+B7)/(B7+B11+B15)</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
väike parandus biti ajastuse arvutamise tekstis
</commit_message>
<xml_diff>
--- a/Software/LowLevel/Documents/bit time.xlsx
+++ b/Software/LowLevel/Documents/bit time.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="16275" windowHeight="5190"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="16275" windowHeight="5190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="F4Disc" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
   <si>
     <t>CAN bit timing on STM32 F4 Discovery kit</t>
   </si>
@@ -75,19 +75,16 @@
     <t>CAN bit timing on STM32 F103 based Robotex microcontroller modules (motor, ball, COMM)</t>
   </si>
   <si>
-    <t>tq = (Prescale + 1) x t PLCK, where Prescale is BRP[9:0] and tplck is APB2 clock</t>
-  </si>
-  <si>
     <t>tq = (Prescale + 1) x t PLCK, where Prescale is BRP[9:0] and tplck is APB1 clock</t>
   </si>
   <si>
     <t>APB1 clokc is system clock / prescale -&gt; 168 Mhz / 4 -&gt; 42 Mhz</t>
   </si>
   <si>
-    <t>APB2 clokc is system clock / prescale -&gt; 48 Mhz / 2 -&gt; 24 Mhz</t>
-  </si>
-  <si>
     <t>sample point %</t>
+  </si>
+  <si>
+    <t>APB1 clock is system clock / prescale -&gt; 48 Mhz / 2 -&gt; 24 Mhz</t>
   </si>
 </sst>
 </file>
@@ -463,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,12 +473,12 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -606,7 +603,7 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -632,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +772,7 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>